<commit_message>
further analysis of low performing boys
</commit_message>
<xml_diff>
--- a/codebook/codebook_covariates_PISA.xlsx
+++ b/codebook/codebook_covariates_PISA.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/PISA_Revisited/codebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9AA0A0-6BFE-7340-BF52-0C21861FE4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BA930D-634C-5B42-81D9-62C506973D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14140" xr2:uid="{D2C9C3A6-3278-CC40-954D-8CD85C6E28F9}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14080" activeTab="1" xr2:uid="{D2C9C3A6-3278-CC40-954D-8CD85C6E28F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="377">
   <si>
     <t>About how much time do you usually spend reading for enjoyment?</t>
   </si>
@@ -947,13 +948,232 @@
   </si>
   <si>
     <t>binary</t>
+  </si>
+  <si>
+    <t>Predictors low performing boys</t>
+  </si>
+  <si>
+    <t>﻿</t>
+  </si>
+  <si>
+    <t>feature</t>
+  </si>
+  <si>
+    <t>coefficient</t>
+  </si>
+  <si>
+    <t>[-19.2902699]</t>
+  </si>
+  <si>
+    <t>[-13.89527142]</t>
+  </si>
+  <si>
+    <t>[13.19525727]</t>
+  </si>
+  <si>
+    <t>[11.79397223]</t>
+  </si>
+  <si>
+    <t>[-11.49530164]</t>
+  </si>
+  <si>
+    <t>[10.76582074]</t>
+  </si>
+  <si>
+    <t>[10.45005645]</t>
+  </si>
+  <si>
+    <t>[9.93586001]</t>
+  </si>
+  <si>
+    <t>[8.65480287]</t>
+  </si>
+  <si>
+    <t>[8.55682094]</t>
+  </si>
+  <si>
+    <t>[8.3704307]</t>
+  </si>
+  <si>
+    <t>[8.26806199]</t>
+  </si>
+  <si>
+    <t>[-8.13531528]</t>
+  </si>
+  <si>
+    <t>[-7.73264355]</t>
+  </si>
+  <si>
+    <t>[-7.65114343]</t>
+  </si>
+  <si>
+    <t>[7.48772601]</t>
+  </si>
+  <si>
+    <t>[7.46018317]</t>
+  </si>
+  <si>
+    <t>[-7.40832298]</t>
+  </si>
+  <si>
+    <t>[7.34422476]</t>
+  </si>
+  <si>
+    <t>ST007Q01TA_5.0</t>
+  </si>
+  <si>
+    <t>[-7.25649332]</t>
+  </si>
+  <si>
+    <t>[7.24345106]</t>
+  </si>
+  <si>
+    <t>[-7.11098691]</t>
+  </si>
+  <si>
+    <t>[6.92684654]</t>
+  </si>
+  <si>
+    <t>[-6.75018957]</t>
+  </si>
+  <si>
+    <t>[6.71586505]</t>
+  </si>
+  <si>
+    <t>[-6.54660294]</t>
+  </si>
+  <si>
+    <t>[-6.41928545]</t>
+  </si>
+  <si>
+    <t>[-6.09391411]</t>
+  </si>
+  <si>
+    <t>[-6.0326206]</t>
+  </si>
+  <si>
+    <t>[5.92453134]</t>
+  </si>
+  <si>
+    <t>[5.68234842]</t>
+  </si>
+  <si>
+    <t>[5.63232331]</t>
+  </si>
+  <si>
+    <t>ST007Q01TA_1.0</t>
+  </si>
+  <si>
+    <t>[5.58437772]</t>
+  </si>
+  <si>
+    <t>[-5.5568185]</t>
+  </si>
+  <si>
+    <t>[-5.3032442]</t>
+  </si>
+  <si>
+    <t>[-5.28952837]</t>
+  </si>
+  <si>
+    <t>[5.26777252]</t>
+  </si>
+  <si>
+    <t>[-5.23373496]</t>
+  </si>
+  <si>
+    <t>[-5.22302117]</t>
+  </si>
+  <si>
+    <t>[-4.76788735]</t>
+  </si>
+  <si>
+    <t>[4.75045719]</t>
+  </si>
+  <si>
+    <t>[4.48620263]</t>
+  </si>
+  <si>
+    <t>ST007Q01TA_2.0</t>
+  </si>
+  <si>
+    <t>[4.40315063]</t>
+  </si>
+  <si>
+    <t>[-4.34950427]</t>
+  </si>
+  <si>
+    <t>[4.33902813]</t>
+  </si>
+  <si>
+    <t>[-4.27372208]</t>
+  </si>
+  <si>
+    <t>[-4.22716997]</t>
+  </si>
+  <si>
+    <t>[-3.96028579]</t>
+  </si>
+  <si>
+    <t>[3.9111231]</t>
+  </si>
+  <si>
+    <t>[-3.8027929]</t>
+  </si>
+  <si>
+    <t>ST005Q01TA_5.0</t>
+  </si>
+  <si>
+    <t>[-3.7213152]</t>
+  </si>
+  <si>
+    <t>ST005Q01TA_1.0</t>
+  </si>
+  <si>
+    <t>[3.66010337]</t>
+  </si>
+  <si>
+    <t>[-3.55600205]</t>
+  </si>
+  <si>
+    <t>[3.54489485]</t>
+  </si>
+  <si>
+    <t>[-3.30988954]</t>
+  </si>
+  <si>
+    <t>[-3.2641313]</t>
+  </si>
+  <si>
+    <t>[3.14129046]</t>
+  </si>
+  <si>
+    <t>[-3.0846373]</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>books at home seem to be the critical point anymore in digital age</t>
+  </si>
+  <si>
+    <t>access to internet on several devices (also ebooks) becomes more important</t>
+  </si>
+  <si>
+    <t>Parents' and teachers' support</t>
+  </si>
+  <si>
+    <t>...here lowest answer (?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -985,16 +1205,49 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1002,16 +1255,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1328,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB48567-618C-9045-84DF-E7AAA47180B4}">
   <dimension ref="A1:E118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3466,4 +3770,923 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9174287B-052F-1D41-9055-5910EEE5EB63}">
+  <dimension ref="A1:R61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="16" t="s">
+        <v>304</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>110</v>
+      </c>
+      <c r="B4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" t="s">
+        <v>308</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>311</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D8" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" t="s">
+        <v>313</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>314</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>81</v>
+      </c>
+      <c r="B11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" t="s">
+        <v>315</v>
+      </c>
+      <c r="D11" t="s">
+        <v>176</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>372</v>
+      </c>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>316</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>317</v>
+      </c>
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>102</v>
+      </c>
+      <c r="B14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C14" t="s">
+        <v>318</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="M14" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>101</v>
+      </c>
+      <c r="B15" t="s">
+        <v>215</v>
+      </c>
+      <c r="C15" t="s">
+        <v>319</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>104</v>
+      </c>
+      <c r="B16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C16" t="s">
+        <v>320</v>
+      </c>
+      <c r="D16" t="s">
+        <v>223</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>321</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>82</v>
+      </c>
+      <c r="B18" t="s">
+        <v>177</v>
+      </c>
+      <c r="C18" t="s">
+        <v>322</v>
+      </c>
+      <c r="D18" t="s">
+        <v>178</v>
+      </c>
+      <c r="M18" s="7"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>323</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>85</v>
+      </c>
+      <c r="B20" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" t="s">
+        <v>324</v>
+      </c>
+      <c r="D20" t="s">
+        <v>184</v>
+      </c>
+      <c r="M20" s="7"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" t="s">
+        <v>325</v>
+      </c>
+      <c r="D21" t="s">
+        <v>85</v>
+      </c>
+      <c r="M21" s="7"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" t="s">
+        <v>326</v>
+      </c>
+      <c r="D22" t="s">
+        <v>196</v>
+      </c>
+      <c r="M22" s="7"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>199</v>
+      </c>
+      <c r="B23" t="s">
+        <v>327</v>
+      </c>
+      <c r="C23" t="s">
+        <v>328</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="J23" t="s">
+        <v>376</v>
+      </c>
+      <c r="M23" s="7"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>329</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C25" t="s">
+        <v>330</v>
+      </c>
+      <c r="D25" t="s">
+        <v>149</v>
+      </c>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" t="s">
+        <v>331</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
+        <v>167</v>
+      </c>
+      <c r="C27" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>105</v>
+      </c>
+      <c r="B32" t="s">
+        <v>224</v>
+      </c>
+      <c r="C32" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>86</v>
+      </c>
+      <c r="B33" t="s">
+        <v>185</v>
+      </c>
+      <c r="C33" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>97</v>
+      </c>
+      <c r="B35" t="s">
+        <v>207</v>
+      </c>
+      <c r="C35" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>195</v>
+      </c>
+      <c r="B36" t="s">
+        <v>341</v>
+      </c>
+      <c r="C36" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>96</v>
+      </c>
+      <c r="B37" t="s">
+        <v>205</v>
+      </c>
+      <c r="C37" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>50</v>
+      </c>
+      <c r="B38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>108</v>
+      </c>
+      <c r="B39" t="s">
+        <v>230</v>
+      </c>
+      <c r="C39" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>14</v>
+      </c>
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>24</v>
+      </c>
+      <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>98</v>
+      </c>
+      <c r="B42" t="s">
+        <v>209</v>
+      </c>
+      <c r="C42" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>57</v>
+      </c>
+      <c r="B43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>58</v>
+      </c>
+      <c r="B44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C44" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>66</v>
+      </c>
+      <c r="B45" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>196</v>
+      </c>
+      <c r="B46" t="s">
+        <v>352</v>
+      </c>
+      <c r="C46" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>37</v>
+      </c>
+      <c r="B47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>69</v>
+      </c>
+      <c r="B48" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>42</v>
+      </c>
+      <c r="B49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>64</v>
+      </c>
+      <c r="B50" t="s">
+        <v>142</v>
+      </c>
+      <c r="C50" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>54</v>
+      </c>
+      <c r="B51" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>89</v>
+      </c>
+      <c r="B52" t="s">
+        <v>191</v>
+      </c>
+      <c r="C52" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>41</v>
+      </c>
+      <c r="B53" t="s">
+        <v>96</v>
+      </c>
+      <c r="C53" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>194</v>
+      </c>
+      <c r="B54" t="s">
+        <v>361</v>
+      </c>
+      <c r="C54" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>190</v>
+      </c>
+      <c r="B55" t="s">
+        <v>363</v>
+      </c>
+      <c r="C55" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>63</v>
+      </c>
+      <c r="B56" t="s">
+        <v>140</v>
+      </c>
+      <c r="C56" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>61</v>
+      </c>
+      <c r="B57" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>44</v>
+      </c>
+      <c r="B58" t="s">
+        <v>102</v>
+      </c>
+      <c r="C58" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>19</v>
+      </c>
+      <c r="B59" t="s">
+        <v>46</v>
+      </c>
+      <c r="C59" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>109</v>
+      </c>
+      <c r="B60" t="s">
+        <v>232</v>
+      </c>
+      <c r="C60" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>73</v>
+      </c>
+      <c r="B61" t="s">
+        <v>159</v>
+      </c>
+      <c r="C61" t="s">
+        <v>370</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>